<commit_message>
timer tests without dups done
</commit_message>
<xml_diff>
--- a/testresults(timer).xlsx
+++ b/testresults(timer).xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav Vachhani\Downloads\SEM-5\CAB301\Assignment 2\Assignment2\CAB301-Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B378BF-4EF2-4099-911B-4112389FF318}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094F19EC-0926-4F06-83D2-A223DAB71893}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E3ACA9F-CD8F-40A6-AD96-15A216C453F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E3ACA9F-CD8F-40A6-AD96-15A216C453F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>timer 1(minDistance)</t>
   </si>
@@ -43,6 +44,18 @@
   </si>
   <si>
     <t>y(theory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array Size </t>
+  </si>
+  <si>
+    <t>Timer 1(minDistance)</t>
+  </si>
+  <si>
+    <t>Timer 2(minDistance2)</t>
+  </si>
+  <si>
+    <t>y(thoery)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +145,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Arrazy Size vs Timer </a:t>
+              <a:t>Array Size vs Timer </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1181,7 +1194,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1303,7 +1316,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1319,6 +1332,1393 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="853380127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Array Size vs Timer </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Timer 1(minDistance)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Timer 1(minDistance)</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4901997138083632E-2"/>
+                  <c:y val="-4.1872785003018595E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1200" baseline="0"/>
+                      <a:t>y = 2E-05x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1200" baseline="30000"/>
+                      <a:t>1.9794</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-AU" sz="1200"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5725</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3589</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4767</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4486</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2845</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3746</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10156</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13276</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7471</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6203</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13715</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9086</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8560</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7295</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14572</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7324</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14194</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6679</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1426</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2556</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2878</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>965</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3116</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3079</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-530E-47B0-A23C-D139B3491C74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Timer 2(minDistance2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Timer 2(minDistance2)</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.3551721157619376E-2"/>
+                  <c:y val="5.6812468495843552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 1E-05x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>1.9436</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5725</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3589</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4767</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4486</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2845</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3746</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10156</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13276</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7471</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6203</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13715</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9086</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8560</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7295</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14572</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7324</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14194</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6679</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1442</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1242</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-530E-47B0-A23C-D139B3491C74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y(thoery)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>y (thoery)</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8396052463403484E-2"/>
+                  <c:y val="6.9166354205724284E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+                      <a:t>y = 3E-05x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1100" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-AU" sz="1100"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5725</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3589</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4767</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4486</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2845</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3746</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10156</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13276</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7471</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6203</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13715</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9086</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8560</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7295</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14572</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7324</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14194</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6679</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13452</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>242.30892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104.01132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>575.53200000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>983.26875000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>978.46563000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.56507000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>386.42763000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>681.72866999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>561.42827999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>432.74412000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>603.72587999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>242.82075</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>631.21707000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>420.97548</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.151679999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3094.3300800000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5287.5652799999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1473.78243</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1674.47523</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1154.31627</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5643.0367500000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2476.6618800000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2198.2080000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1596.5107500000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6370.2955200000006</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1609.22928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6044.0890799999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1338.2712300000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5428.68912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-530E-47B0-A23C-D139B3491C74}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="216612383"/>
+        <c:axId val="353994175"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="216612383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Array Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353994175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="353994175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Timee taken to execute (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="216612383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1438,7 +2838,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1975,6 +3931,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D9B763-1FF6-47F5-B759-4425096E1574}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CE3144-0963-4E99-91EB-5E1B03C8E9FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2294,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A70A97-ED3E-460C-887F-896418341F50}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,4 +4755,474 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF91067-CD29-4D07-8FCC-F2C96EEE03E9}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2842</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>55</v>
+      </c>
+      <c r="D2">
+        <f>0.00003*(A2*A2)</f>
+        <v>242.30892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1862</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D30" si="0">0.00003*(A3*A3)</f>
+        <v>104.01132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4380</v>
+      </c>
+      <c r="B4">
+        <v>256</v>
+      </c>
+      <c r="C4">
+        <v>131</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>575.53200000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5725</v>
+      </c>
+      <c r="B5">
+        <v>439</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>983.26875000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5711</v>
+      </c>
+      <c r="B6">
+        <v>429</v>
+      </c>
+      <c r="C6">
+        <v>221</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>978.46563000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2013</v>
+      </c>
+      <c r="B7">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>121.56507000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3589</v>
+      </c>
+      <c r="B8">
+        <v>171</v>
+      </c>
+      <c r="C8">
+        <v>87</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>386.42763000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4767</v>
+      </c>
+      <c r="B9">
+        <v>307</v>
+      </c>
+      <c r="C9">
+        <v>158</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>681.72866999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4326</v>
+      </c>
+      <c r="B10">
+        <v>251</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>561.42827999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3798</v>
+      </c>
+      <c r="B11">
+        <v>188</v>
+      </c>
+      <c r="C11">
+        <v>97</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>432.74412000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4486</v>
+      </c>
+      <c r="B12">
+        <v>272</v>
+      </c>
+      <c r="C12">
+        <v>139</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>603.72587999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2845</v>
+      </c>
+      <c r="B13">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>242.82075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4587</v>
+      </c>
+      <c r="B14">
+        <v>355</v>
+      </c>
+      <c r="C14">
+        <v>251</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>631.21707000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3746</v>
+      </c>
+      <c r="B15">
+        <v>279</v>
+      </c>
+      <c r="C15">
+        <v>143</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>420.97548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1416</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>60.151679999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10156</v>
+      </c>
+      <c r="B17">
+        <v>1426</v>
+      </c>
+      <c r="C17">
+        <v>709</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>3094.3300800000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13276</v>
+      </c>
+      <c r="B18">
+        <v>2556</v>
+      </c>
+      <c r="C18">
+        <v>1193</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5287.5652799999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7009</v>
+      </c>
+      <c r="B19">
+        <v>690</v>
+      </c>
+      <c r="C19">
+        <v>331</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1473.78243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7471</v>
+      </c>
+      <c r="B20">
+        <v>733</v>
+      </c>
+      <c r="C20">
+        <v>376</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1674.47523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6203</v>
+      </c>
+      <c r="B21">
+        <v>510</v>
+      </c>
+      <c r="C21">
+        <v>256</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1154.31627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13715</v>
+      </c>
+      <c r="B22">
+        <v>2878</v>
+      </c>
+      <c r="C22">
+        <v>1340</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>5643.0367500000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9086</v>
+      </c>
+      <c r="B23">
+        <v>1090</v>
+      </c>
+      <c r="C23">
+        <v>714</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2476.6618800000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8560</v>
+      </c>
+      <c r="B24">
+        <v>965</v>
+      </c>
+      <c r="C24">
+        <v>498</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2198.2080000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7295</v>
+      </c>
+      <c r="B25">
+        <v>710</v>
+      </c>
+      <c r="C25">
+        <v>360</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1596.5107500000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14572</v>
+      </c>
+      <c r="B26">
+        <v>3116</v>
+      </c>
+      <c r="C26">
+        <v>1442</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>6370.2955200000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7324</v>
+      </c>
+      <c r="B27">
+        <v>707</v>
+      </c>
+      <c r="C27">
+        <v>367</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1609.22928</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>14194</v>
+      </c>
+      <c r="B28">
+        <v>3079</v>
+      </c>
+      <c r="C28">
+        <v>1416</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>6044.0890799999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6679</v>
+      </c>
+      <c r="B29">
+        <v>595</v>
+      </c>
+      <c r="C29">
+        <v>308</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1338.2712300000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>13452</v>
+      </c>
+      <c r="B30">
+        <v>2611</v>
+      </c>
+      <c r="C30">
+        <v>1242</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>5428.68912</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>